<commit_message>
Extend .set to take an array of array or nested object
</commit_message>
<xml_diff>
--- a/test/out/image-png.xlsx
+++ b/test/out/image-png.xlsx
@@ -69,15 +69,15 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>0</xdr:col>
+      <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>0</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
+      <xdr:col>7</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -98,6 +98,9 @@
           <a:extLst>
             <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
               <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+            <a:ext uri="{96DAC541-7B7A-43D3-8B79-37D633B846F1}">
+              <asvg:svgBlip xmlns:asvg="http://schemas.microsoft.com/office/drawing/2016/SVG/main" r:embed="rId1"/>
             </a:ext>
           </a:extLst>
         </a:blip>

</xml_diff>